<commit_message>
Client can be updated
Update client
</commit_message>
<xml_diff>
--- a/public/OFFICE STRUCTURE.xlsx
+++ b/public/OFFICE STRUCTURE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashbeemorgado/devs/laf/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1701A052-4A5A-644E-864C-DF41642E571E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F972BC2A-FC6A-9946-AAA3-D712D0603241}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20560" xr2:uid="{B219841F-3218-4145-B920-CF973D62632C}"/>
+    <workbookView xWindow="20060" yWindow="500" windowWidth="15780" windowHeight="20560" xr2:uid="{B219841F-3218-4145-B920-CF973D62632C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4339,7 +4339,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -4362,26 +4362,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4700,10 +4688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45A1E2B0-13DC-394E-86C0-419AFE350589}">
-  <dimension ref="A1:J1339"/>
+  <dimension ref="A1:G1339"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1265" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E1285" sqref="A1285:E1339"/>
+    <sheetView tabSelected="1" topLeftCell="A315" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4712,119 +4700,116 @@
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="44" max="45" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="14" bestFit="1" customWidth="1"/>
-    <col min="56" max="57" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="14" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="13" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="42" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="14" bestFit="1" customWidth="1"/>
+    <col min="57" max="58" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="13" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="14" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="14" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="19" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="19" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="19" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="20" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="18" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="19" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="17" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="19" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="16" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="19" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="15" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="19" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="19" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="19" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="19" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="20" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="18" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="19" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="17" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="19" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="16" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="19" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="15" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="19" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -4841,7 +4826,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4858,7 +4843,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4875,7 +4860,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4892,7 +4877,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4909,7 +4894,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4926,7 +4911,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4943,7 +4928,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4960,7 +4945,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4977,7 +4962,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4994,7 +4979,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -5011,7 +4996,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -5028,7 +5013,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -5045,7 +5030,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -5062,7 +5047,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -5078,9 +5063,9 @@
       <c r="E15" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -5097,7 +5082,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -5114,7 +5099,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -5131,7 +5116,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -5147,11 +5132,8 @@
       <c r="E19" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -5168,7 +5150,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -5185,7 +5167,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -5202,7 +5184,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -5219,7 +5201,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -5236,7 +5218,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -5253,7 +5235,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -5270,7 +5252,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -5287,7 +5269,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -5304,7 +5286,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -5321,7 +5303,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -5338,7 +5320,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -5355,7 +5337,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>

</xml_diff>